<commit_message>
Apply 1% winsorization to ln_carbon_intensity dependent variable
Changes:
- Added 1% winsorization on ln_碳排放强度 (1% and 99% percentiles)
- 66 observations adjusted (2.02% of sample)
- Winsorization bounds: lower=8.2654, upper=11.6941

Results comparison:
- Before winsorization: DID=0.0603*** (6.22% increase)
- After winsorization: DID=0.0553*** (5.69% increase)
- Coefficient decreased by 8.3% due to outlier treatment

Interpretation:
Policy still has significant positive effect on carbon intensity
(p<0.01), suggesting pilot cities had 5.69% higher carbon
intensity compared to control cities after policy implementation.
</commit_message>
<xml_diff>
--- a/did_multiperiod/results/twfe_coefficients.xlsx
+++ b/did_multiperiod/results/twfe_coefficients.xlsx
@@ -472,16 +472,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.02002320484287e-16</v>
+        <v>-1.027810138928968e-15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002483133269656471</v>
+        <v>0.002482392527945528</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.107806928075132e-14</v>
+        <v>-4.140401356185205e-13</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9999999999999671</v>
+        <v>0.9999999999996698</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06030746612179659</v>
+        <v>0.05532890472139857</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01053830287239001</v>
+        <v>0.01053515919879201</v>
       </c>
       <c r="D3" t="n">
-        <v>5.722692434642403</v>
+        <v>5.251833757551831</v>
       </c>
       <c r="E3" t="n">
-        <v>1.143439698481075e-08</v>
+        <v>1.602573171943789e-07</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -516,13 +516,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.8015559143991771</v>
+        <v>-0.8092585493269315</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04224137516880389</v>
+        <v>0.04222877417436777</v>
       </c>
       <c r="D4" t="n">
-        <v>-18.97561126255999</v>
+        <v>-19.16367607511893</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -540,16 +540,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.04740845349318212</v>
+        <v>-0.0188714528127612</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03673721375387445</v>
+        <v>0.03672625470189612</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.290474933967529</v>
+        <v>-0.5138409284022881</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1969773835288764</v>
+        <v>0.607398056844755</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -560,16 +560,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03211836097861366</v>
+        <v>0.01107475954305597</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01993151079527508</v>
+        <v>0.01992556504053506</v>
       </c>
       <c r="D6" t="n">
-        <v>1.611436348629807</v>
+        <v>0.5558065490502437</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1071815137911454</v>
+        <v>0.5783812727909732</v>
       </c>
       <c r="F6" t="inlineStr"/>
     </row>
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3095160032070732</v>
+        <v>0.2940073584038606</v>
       </c>
       <c r="C7" t="n">
-        <v>0.066160534102349</v>
+        <v>0.06614079780070675</v>
       </c>
       <c r="D7" t="n">
-        <v>4.678257323743159</v>
+        <v>4.445174055652515</v>
       </c>
       <c r="E7" t="n">
-        <v>3.010958036453459e-06</v>
+        <v>9.074980176437819e-06</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>

</xml_diff>